<commit_message>
Finding By css selector and xpath
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{CE106356-CD68-43BE-9697-3CF8F299211C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33C6AC33-2565-48F0-BC4E-FBE4D53AC715}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="1800" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -293,6 +293,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -560,9 +564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>